<commit_message>
Feat: 리소스 close 수정
</commit_message>
<xml_diff>
--- a/members.xlsx
+++ b/members.xlsx
@@ -35,13 +35,13 @@
     <t>lee</t>
   </si>
   <si>
-    <t>lawejg</t>
+    <t>dsfj</t>
   </si>
   <si>
-    <t>2384719</t>
+    <t>234</t>
   </si>
   <si>
-    <t>fjkdsh</t>
+    <t>kf</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>124235.0</v>
+        <v>12.0</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>

</xml_diff>